<commit_message>
Update - DistanceMatriz and PCA.
</commit_message>
<xml_diff>
--- a/DataIntermediate/resultados_regresiones.xlsx
+++ b/DataIntermediate/resultados_regresiones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="R2" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="R2 Ajustado" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="P-Values" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Regresiones con R2 &gt; 0.1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R2 Ajustado" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="P-Values" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Regresiones con R2 &gt; 0.1" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1633797165198528</v>
+        <v>0.1633797165198531</v>
       </c>
     </row>
     <row r="3">
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.268174153801026</v>
+        <v>0.2681741538010264</v>
       </c>
     </row>
     <row r="6">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.23274428111255</v>
+        <v>0.2327442811125501</v>
       </c>
     </row>
     <row r="7">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.3487128187823491</v>
+        <v>0.3487128187823492</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1583347564598894</v>
+        <v>0.1583347564598896</v>
       </c>
     </row>
     <row r="10">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.01887257664600928</v>
+        <v>0.01887257664600961</v>
       </c>
     </row>
     <row r="3">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1417678712757489</v>
+        <v>0.1417678712757492</v>
       </c>
     </row>
     <row r="6">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1002182933047178</v>
+        <v>0.1002182933047179</v>
       </c>
     </row>
     <row r="7">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2362177602083912</v>
+        <v>0.2362177602083914</v>
       </c>
     </row>
     <row r="9">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0129562143938704</v>
+        <v>0.01295621439387062</v>
       </c>
     </row>
     <row r="10">
@@ -689,64 +689,64 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>4.00755247427068e-05</v>
+        <v>4.00755247427071e-05</v>
       </c>
       <c r="C1" t="n">
-        <v>0.7068379325017994</v>
+        <v>0.7068379325017954</v>
       </c>
       <c r="D1" t="n">
-        <v>0.02992983341058821</v>
+        <v>0.02992983341058839</v>
       </c>
       <c r="E1" t="n">
-        <v>0.1407262542433185</v>
+        <v>0.1407262542433192</v>
       </c>
       <c r="F1" t="n">
-        <v>0.2742584340714386</v>
+        <v>0.2742584340714384</v>
       </c>
       <c r="G1" t="n">
-        <v>0.9102224425934142</v>
+        <v>0.910222442593408</v>
       </c>
       <c r="H1" t="n">
-        <v>0.5169380628818115</v>
+        <v>0.5169380628818178</v>
       </c>
       <c r="I1" t="n">
-        <v>0.4509907377012583</v>
+        <v>0.4509907377012581</v>
       </c>
       <c r="J1" t="n">
-        <v>0.0409474435643237</v>
+        <v>0.04094744356432451</v>
       </c>
       <c r="K1" t="n">
-        <v>0.6004784490284638</v>
+        <v>0.6004784490284686</v>
       </c>
       <c r="L1" t="n">
-        <v>0.2367454733067574</v>
+        <v>0.2367454733067542</v>
       </c>
       <c r="M1" t="n">
-        <v>0.0884223339325132</v>
+        <v>0.0884223339325131</v>
       </c>
       <c r="N1" t="n">
-        <v>0.6890166017581263</v>
+        <v>0.6890166017581282</v>
       </c>
       <c r="O1" t="n">
-        <v>0.8374363546028417</v>
+        <v>0.8374363546028423</v>
       </c>
       <c r="P1" t="n">
-        <v>0.6738285520833698</v>
+        <v>0.673828552083367</v>
       </c>
       <c r="Q1" t="n">
-        <v>0.5761682740985652</v>
+        <v>0.5761682740985654</v>
       </c>
       <c r="R1" t="n">
-        <v>0.003269936357667117</v>
+        <v>0.003269936357667177</v>
       </c>
       <c r="S1" t="n">
-        <v>0.1986556256475436</v>
+        <v>0.1986556256475429</v>
       </c>
       <c r="T1" t="n">
-        <v>0.6406648697044905</v>
+        <v>0.6406648697044867</v>
       </c>
       <c r="U1" t="n">
-        <v>0.2081041820332367</v>
+        <v>0.2081041820332391</v>
       </c>
     </row>
     <row r="2">
@@ -756,64 +756,64 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.002645074185903675</v>
+        <v>0.002645074185903679</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03218198245488626</v>
+        <v>0.03218198245488594</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4080310479324237</v>
+        <v>0.4080310479324254</v>
       </c>
       <c r="E2" t="n">
         <v>0.0453073229977929</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5001616827108746</v>
+        <v>0.5001616827108711</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5400448440232457</v>
+        <v>0.5400448440232533</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8634415609421445</v>
+        <v>0.8634415609421537</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5283717545349889</v>
+        <v>0.5283717545349902</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8769124218674813</v>
+        <v>0.8769124218674806</v>
       </c>
       <c r="K2" t="n">
-        <v>0.05110513998194765</v>
+        <v>0.05110513998194839</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6261413330681069</v>
+        <v>0.6261413330680945</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1854692753008992</v>
+        <v>0.185469275300898</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2999922334886875</v>
+        <v>0.2999922334886886</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8089445983036034</v>
+        <v>0.8089445983036048</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1846882199301716</v>
+        <v>0.1846882199301725</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4788096445990004</v>
+        <v>0.4788096445990003</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7256974496700095</v>
+        <v>0.7256974496700122</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7227637024500109</v>
+        <v>0.7227637024500115</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9813288506846931</v>
+        <v>0.9813288506846876</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9060043835222564</v>
+        <v>0.9060043835222512</v>
       </c>
     </row>
     <row r="3">
@@ -823,64 +823,64 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9945688118866688</v>
+        <v>0.9945688118866698</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7926788323681966</v>
+        <v>0.7926788323681933</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3243341118915266</v>
+        <v>0.3243341118915276</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9005073870947169</v>
+        <v>0.900507387094717</v>
       </c>
       <c r="F3" t="n">
-        <v>0.179977969045673</v>
+        <v>0.1799779690456735</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06011532677852329</v>
+        <v>0.06011532677852445</v>
       </c>
       <c r="H3" t="n">
-        <v>0.05870557222267388</v>
+        <v>0.05870557222267347</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6729548651802879</v>
+        <v>0.6729548651802877</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7330931233943021</v>
+        <v>0.7330931233943059</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1400657213069368</v>
+        <v>0.1400657213069377</v>
       </c>
       <c r="L3" t="n">
-        <v>0.04490455557264588</v>
+        <v>0.04490455557264642</v>
       </c>
       <c r="M3" t="n">
-        <v>0.007946613137866923</v>
+        <v>0.007946613137866897</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2513240139996692</v>
+        <v>0.2513240139996701</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2088406038553605</v>
+        <v>0.2088406038553618</v>
       </c>
       <c r="P3" t="n">
-        <v>0.741655837740905</v>
+        <v>0.7416558377409055</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8379011190353234</v>
+        <v>0.8379011190353207</v>
       </c>
       <c r="R3" t="n">
-        <v>0.08323944181620262</v>
+        <v>0.08323944181620309</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9475644119678605</v>
+        <v>0.9475644119678593</v>
       </c>
       <c r="T3" t="n">
-        <v>0.05988653500434928</v>
+        <v>0.05988653500434948</v>
       </c>
       <c r="U3" t="n">
-        <v>0.6163599298820017</v>
+        <v>0.6163599298820009</v>
       </c>
     </row>
     <row r="4">
@@ -890,64 +890,64 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5369493879595882</v>
+        <v>0.5369493879595879</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2830907615378621</v>
+        <v>0.2830907615378633</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8215877221209352</v>
+        <v>0.8215877221209388</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8438003832547893</v>
+        <v>0.8438003832547869</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2559991894965702</v>
+        <v>0.255999189496571</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09559344493621917</v>
+        <v>0.09559344493622066</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6278907063985707</v>
+        <v>0.6278907063985727</v>
       </c>
       <c r="I4" t="n">
-        <v>0.565051521893057</v>
+        <v>0.5650515218930572</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2794578274342027</v>
+        <v>0.2794578274342044</v>
       </c>
       <c r="K4" t="n">
-        <v>0.186637373533238</v>
+        <v>0.1866373735332381</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5002643462601555</v>
+        <v>0.5002643462601564</v>
       </c>
       <c r="M4" t="n">
-        <v>0.05533256693296051</v>
+        <v>0.05533256693296055</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0006896482744836326</v>
+        <v>0.0006896482744836373</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2808853731145509</v>
+        <v>0.2808853731145511</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0164098066453841</v>
+        <v>0.01640980664538396</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.3093144483030168</v>
+        <v>0.3093144483030159</v>
       </c>
       <c r="R4" t="n">
-        <v>0.2034135165970737</v>
+        <v>0.2034135165970749</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8892740555109873</v>
+        <v>0.8892740555109864</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9399952780579691</v>
+        <v>0.9399952780579717</v>
       </c>
       <c r="U4" t="n">
-        <v>0.06782885886504919</v>
+        <v>0.06782885886504907</v>
       </c>
     </row>
     <row r="5">
@@ -957,64 +957,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6117942391759907</v>
+        <v>0.6117942391759921</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1487968486895587</v>
+        <v>0.1487968486895597</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2340228302688486</v>
+        <v>0.2340228302688489</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9072863429668818</v>
+        <v>0.9072863429668848</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4445966546326785</v>
+        <v>0.4445966546326808</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8922732827386454</v>
+        <v>0.8922732827386483</v>
       </c>
       <c r="H5" t="n">
-        <v>0.05718300138255247</v>
+        <v>0.05718300138255217</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3200439573441765</v>
+        <v>0.3200439573441771</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8669316763264272</v>
+        <v>0.866931676326423</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6912954455932816</v>
+        <v>0.6912954455932823</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7421999256642107</v>
+        <v>0.7421999256642098</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0008769435082888492</v>
+        <v>0.0008769435082888595</v>
       </c>
       <c r="N5" t="n">
-        <v>0.5828988876383969</v>
+        <v>0.5828988876384</v>
       </c>
       <c r="O5" t="n">
-        <v>0.4515817450072788</v>
+        <v>0.4515817450072783</v>
       </c>
       <c r="P5" t="n">
-        <v>0.6749062893461721</v>
+        <v>0.6749062893461719</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.9462462081179833</v>
+        <v>0.9462462081179821</v>
       </c>
       <c r="R5" t="n">
-        <v>0.2845537276839284</v>
+        <v>0.2845537276839289</v>
       </c>
       <c r="S5" t="n">
-        <v>0.3482744816232674</v>
+        <v>0.3482744816232678</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8190187501833202</v>
+        <v>0.8190187501833215</v>
       </c>
       <c r="U5" t="n">
-        <v>0.4014438992086047</v>
+        <v>0.401443899208605</v>
       </c>
     </row>
     <row r="6">
@@ -1024,64 +1024,64 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3173360395885775</v>
+        <v>0.3173360395885771</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8986921529264688</v>
+        <v>0.8986921529264735</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3802999228835977</v>
+        <v>0.3802999228835987</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4624299886525489</v>
+        <v>0.4624299886525474</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4286283719146109</v>
+        <v>0.4286283719146096</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6569020775370265</v>
+        <v>0.6569020775370316</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5853751264808764</v>
+        <v>0.5853751264808792</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9776302429834707</v>
+        <v>0.9776302429834713</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3126082993895312</v>
+        <v>0.3126082993895299</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9513363615709008</v>
+        <v>0.9513363615709037</v>
       </c>
       <c r="L6" t="n">
-        <v>0.6611841476526144</v>
+        <v>0.6611841476526106</v>
       </c>
       <c r="M6" t="n">
-        <v>0.02316269948786348</v>
+        <v>0.02316269948786338</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1712285298202679</v>
+        <v>0.1712285298202687</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3077687013513086</v>
+        <v>0.307768701351309</v>
       </c>
       <c r="P6" t="n">
-        <v>0.7684476159637209</v>
+        <v>0.7684476159637179</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.6174393891886292</v>
+        <v>0.6174393891886316</v>
       </c>
       <c r="R6" t="n">
-        <v>0.9833386233623237</v>
+        <v>0.9833386233623264</v>
       </c>
       <c r="S6" t="n">
-        <v>0.543409874324811</v>
+        <v>0.5434098743248124</v>
       </c>
       <c r="T6" t="n">
-        <v>0.3239971864312134</v>
+        <v>0.323997186431213</v>
       </c>
       <c r="U6" t="n">
-        <v>0.9262915079029184</v>
+        <v>0.9262915079029224</v>
       </c>
     </row>
     <row r="7">
@@ -1091,64 +1091,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1624893589915481</v>
+        <v>0.1624893589915478</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8131271284717937</v>
+        <v>0.8131271284717971</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7609034489414657</v>
+        <v>0.7609034489414649</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9714252399703568</v>
+        <v>0.9714252399703591</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1993814590325207</v>
+        <v>0.1993814590325213</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6798848522848402</v>
+        <v>0.6798848522848351</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9117449554434748</v>
+        <v>0.9117449554434793</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7701861506612991</v>
+        <v>0.7701861506612999</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8660588842835131</v>
+        <v>0.8660588842835159</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5612111219428062</v>
+        <v>0.5612111219428091</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1259596451665234</v>
+        <v>0.1259596451665229</v>
       </c>
       <c r="M7" t="n">
         <v>0.02319344635691789</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3154009600794337</v>
+        <v>0.3154009600794341</v>
       </c>
       <c r="O7" t="n">
-        <v>0.6631909894733371</v>
+        <v>0.6631909894733368</v>
       </c>
       <c r="P7" t="n">
-        <v>0.6411364791697726</v>
+        <v>0.6411364791697738</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.3176054189908309</v>
+        <v>0.3176054189908321</v>
       </c>
       <c r="R7" t="n">
-        <v>0.4848775887830613</v>
+        <v>0.4848775887830626</v>
       </c>
       <c r="S7" t="n">
-        <v>0.8426815305802341</v>
+        <v>0.8426815305802335</v>
       </c>
       <c r="T7" t="n">
-        <v>0.5960111730679447</v>
+        <v>0.5960111730679436</v>
       </c>
       <c r="U7" t="n">
-        <v>0.2972179968290932</v>
+        <v>0.2972179968290954</v>
       </c>
     </row>
     <row r="8">
@@ -1158,64 +1158,64 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07209572435745107</v>
+        <v>0.0720957243574515</v>
       </c>
       <c r="C8" t="n">
-        <v>0.05857780415635051</v>
+        <v>0.05857780415635086</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7745033611937048</v>
+        <v>0.7745033611937034</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6099700258092836</v>
+        <v>0.6099700258092876</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3173595518837796</v>
+        <v>0.3173595518837829</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2206882735967188</v>
+        <v>0.2206882735967192</v>
       </c>
       <c r="H8" t="n">
-        <v>0.3833518829521548</v>
+        <v>0.3833518829521563</v>
       </c>
       <c r="I8" t="n">
-        <v>0.04040274805474822</v>
+        <v>0.0404027480547484</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6834028632741747</v>
+        <v>0.6834028632741794</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6026250988249089</v>
+        <v>0.6026250988249078</v>
       </c>
       <c r="L8" t="n">
-        <v>0.4587341480679478</v>
+        <v>0.458734148067951</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0004176458920286368</v>
+        <v>0.0004176458920286408</v>
       </c>
       <c r="N8" t="n">
-        <v>0.09043827455195368</v>
+        <v>0.09043827455195456</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9851419941382917</v>
+        <v>0.985141994138292</v>
       </c>
       <c r="P8" t="n">
-        <v>0.389108326156368</v>
+        <v>0.3891083261563678</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.9000545166320066</v>
+        <v>0.9000545166320074</v>
       </c>
       <c r="R8" t="n">
-        <v>0.6938036783126469</v>
+        <v>0.6938036783126476</v>
       </c>
       <c r="S8" t="n">
-        <v>0.05130456822602498</v>
+        <v>0.05130456822602505</v>
       </c>
       <c r="T8" t="n">
-        <v>0.4825424835263763</v>
+        <v>0.4825424835263791</v>
       </c>
       <c r="U8" t="n">
-        <v>0.2144833143165437</v>
+        <v>0.2144833143165428</v>
       </c>
     </row>
     <row r="9">
@@ -1225,64 +1225,64 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.05502437684639472</v>
+        <v>0.05502437684639464</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6135549197241548</v>
+        <v>0.6135549197241521</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8406509478194866</v>
+        <v>0.8406509478194905</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5087173312499125</v>
+        <v>0.5087173312499108</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3598790231569859</v>
+        <v>0.3598790231569851</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9919075707361245</v>
+        <v>0.9919075707361162</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5153937716698336</v>
+        <v>0.5153937716698385</v>
       </c>
       <c r="I9" t="n">
-        <v>0.3378062818310531</v>
+        <v>0.3378062818310523</v>
       </c>
       <c r="J9" t="n">
-        <v>0.7885180262315477</v>
+        <v>0.7885180262315475</v>
       </c>
       <c r="K9" t="n">
-        <v>0.768471159370316</v>
+        <v>0.768471159370312</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1453935957441724</v>
+        <v>0.1453935957441712</v>
       </c>
       <c r="M9" t="n">
-        <v>0.04833063294771912</v>
+        <v>0.04833063294771878</v>
       </c>
       <c r="N9" t="n">
-        <v>0.286233541297233</v>
+        <v>0.2862335412972336</v>
       </c>
       <c r="O9" t="n">
-        <v>0.5813621941671679</v>
+        <v>0.5813621941671678</v>
       </c>
       <c r="P9" t="n">
-        <v>0.5329551387885265</v>
+        <v>0.5329551387885273</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.3514007776902055</v>
+        <v>0.3514007776902066</v>
       </c>
       <c r="R9" t="n">
-        <v>0.833627445728691</v>
+        <v>0.833627445728694</v>
       </c>
       <c r="S9" t="n">
-        <v>0.9959172035252276</v>
+        <v>0.9959172035252303</v>
       </c>
       <c r="T9" t="n">
-        <v>0.5101741140416747</v>
+        <v>0.5101741140416725</v>
       </c>
       <c r="U9" t="n">
-        <v>0.5744893767829458</v>
+        <v>0.5744893767829417</v>
       </c>
     </row>
     <row r="10">
@@ -1292,64 +1292,64 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3075104910414613</v>
+        <v>0.3075104910414607</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9910845616514836</v>
+        <v>0.9910845616514798</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8077369997119608</v>
+        <v>0.8077369997119616</v>
       </c>
       <c r="E10" t="n">
-        <v>0.823985943646529</v>
+        <v>0.8239859436465266</v>
       </c>
       <c r="F10" t="n">
         <v>0.2838179115371484</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9653593234973439</v>
+        <v>0.9653593234973374</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9534382793861015</v>
+        <v>0.9534382793860976</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8048022899787721</v>
+        <v>0.8048022899787729</v>
       </c>
       <c r="J10" t="n">
-        <v>0.8887035516100513</v>
+        <v>0.8887035516100485</v>
       </c>
       <c r="K10" t="n">
-        <v>0.6391436083720226</v>
+        <v>0.6391436083720252</v>
       </c>
       <c r="L10" t="n">
-        <v>0.3284026431743905</v>
+        <v>0.3284026431743886</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0154267586256702</v>
+        <v>0.0154267586256701</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1194808748395421</v>
+        <v>0.1194808748395428</v>
       </c>
       <c r="O10" t="n">
-        <v>0.3318155584042917</v>
+        <v>0.3318155584042912</v>
       </c>
       <c r="P10" t="n">
-        <v>0.943229817050523</v>
+        <v>0.9432298170505251</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.4332185940664146</v>
+        <v>0.4332185940664164</v>
       </c>
       <c r="R10" t="n">
-        <v>0.9195106766720713</v>
+        <v>0.9195106766720736</v>
       </c>
       <c r="S10" t="n">
-        <v>0.8886747837526893</v>
+        <v>0.8886747837526878</v>
       </c>
       <c r="T10" t="n">
-        <v>0.9770915463813796</v>
+        <v>0.9770915463813787</v>
       </c>
       <c r="U10" t="n">
-        <v>0.2425964393313262</v>
+        <v>0.2425964393313277</v>
       </c>
     </row>
     <row r="11">
@@ -1359,64 +1359,64 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5029240963405994</v>
+        <v>0.5029240963405986</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2658244254283788</v>
+        <v>0.2658244254283789</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6255500975141787</v>
+        <v>0.6255500975141812</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1278369888866854</v>
+        <v>0.1278369888866852</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6248698313132752</v>
+        <v>0.6248698313132768</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5005215247965287</v>
+        <v>0.5005215247965329</v>
       </c>
       <c r="H11" t="n">
-        <v>0.009928920910173448</v>
+        <v>0.009928920910173548</v>
       </c>
       <c r="I11" t="n">
-        <v>0.8270645476751219</v>
+        <v>0.8270645476751211</v>
       </c>
       <c r="J11" t="n">
         <v>0.03744676842325655</v>
       </c>
       <c r="K11" t="n">
-        <v>0.01817297199574427</v>
+        <v>0.01817297199574443</v>
       </c>
       <c r="L11" t="n">
-        <v>0.6608712896262454</v>
+        <v>0.6608712896262432</v>
       </c>
       <c r="M11" t="n">
-        <v>0.101975749143905</v>
+        <v>0.1019757491439043</v>
       </c>
       <c r="N11" t="n">
-        <v>0.5160044928758691</v>
+        <v>0.5160044928758696</v>
       </c>
       <c r="O11" t="n">
-        <v>0.9043140070436173</v>
+        <v>0.9043140070436171</v>
       </c>
       <c r="P11" t="n">
-        <v>0.7346646990324588</v>
+        <v>0.7346646990324607</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.5096575718280116</v>
+        <v>0.5096575718280127</v>
       </c>
       <c r="R11" t="n">
-        <v>0.2022966164003586</v>
+        <v>0.2022966164003593</v>
       </c>
       <c r="S11" t="n">
-        <v>0.8725209695587033</v>
+        <v>0.8725209695587061</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8657335101506271</v>
+        <v>0.8657335101506241</v>
       </c>
       <c r="U11" t="n">
-        <v>0.7757902316331162</v>
+        <v>0.7757902316331157</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1417678712757489</v>
+        <v>0.1417678712757492</v>
       </c>
     </row>
     <row r="6">
@@ -1475,7 +1475,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1002182933047178</v>
+        <v>0.1002182933047179</v>
       </c>
     </row>
     <row r="8">
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2362177602083912</v>
+        <v>0.2362177602083914</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Update - Save the importances of the RF
</commit_message>
<xml_diff>
--- a/DataIntermediate/resultados_regresiones.xlsx
+++ b/DataIntermediate/resultados_regresiones.xlsx
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.314648208393887</v>
+        <v>0.4030976049049029</v>
       </c>
     </row>
     <row r="2">
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2892410690173153</v>
+        <v>0.2892992812609153</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.337763713672747</v>
+        <v>0.3404847182103248</v>
       </c>
     </row>
     <row r="4">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3463414080270697</v>
+        <v>0.3326554295679346</v>
       </c>
     </row>
     <row r="5">
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3607262826801678</v>
+        <v>0.3595556653328901</v>
       </c>
     </row>
     <row r="6">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3892858094266229</v>
+        <v>0.3872376226745848</v>
       </c>
     </row>
     <row r="7">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2952011167710191</v>
+        <v>0.2903928263120256</v>
       </c>
     </row>
     <row r="8">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4107248878397699</v>
+        <v>0.4152753050597068</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.3171669178837616</v>
+        <v>0.3109068240986995</v>
       </c>
     </row>
     <row r="10">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3633650763900297</v>
+        <v>0.3610734442332768</v>
       </c>
     </row>
     <row r="11">
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3425148933864568</v>
+        <v>0.333602005196685</v>
       </c>
     </row>
   </sheetData>
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.1314353532120548</v>
+        <v>0.2435296378992828</v>
       </c>
     </row>
     <row r="2">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0992362062793698</v>
+        <v>0.099309980211853</v>
       </c>
     </row>
     <row r="3">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1607302509912042</v>
+        <v>0.1641786527814016</v>
       </c>
     </row>
     <row r="4">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1716009923511378</v>
+        <v>0.1542563859870855</v>
       </c>
     </row>
     <row r="5">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1898313285451632</v>
+        <v>0.188347773887227</v>
       </c>
     </row>
     <row r="6">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2260255802634429</v>
+        <v>0.2234298584390778</v>
       </c>
     </row>
     <row r="7">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.106789534125648</v>
+        <v>0.1006958590885076</v>
       </c>
     </row>
     <row r="8">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2531958974603025</v>
+        <v>0.2589627628479452</v>
       </c>
     </row>
     <row r="9">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1346273810804107</v>
+        <v>0.1266937968775598</v>
       </c>
     </row>
     <row r="10">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1931755423556811</v>
+        <v>0.1902712956619745</v>
       </c>
     </row>
     <row r="11">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1667515480541235</v>
+        <v>0.1554560065858979</v>
       </c>
     </row>
   </sheetData>
@@ -689,88 +689,88 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.0004139928709682987</v>
+        <v>0.8417814867328168</v>
       </c>
       <c r="C1" t="n">
-        <v>0.1151210208317256</v>
+        <v>0.2636718498637532</v>
       </c>
       <c r="D1" t="n">
-        <v>0.1500656946996005</v>
+        <v>0.3491375520943799</v>
       </c>
       <c r="E1" t="n">
-        <v>0.003896346021540899</v>
+        <v>0.001831926995122671</v>
       </c>
       <c r="F1" t="n">
-        <v>0.01329627721108939</v>
+        <v>0.02952172182074858</v>
       </c>
       <c r="G1" t="n">
-        <v>0.0102766133311377</v>
+        <v>0.007424627989425388</v>
       </c>
       <c r="H1" t="n">
-        <v>0.2484258780735239</v>
+        <v>0.205761112236049</v>
       </c>
       <c r="I1" t="n">
-        <v>0.3950927164990987</v>
+        <v>0.5190950201303681</v>
       </c>
       <c r="J1" t="n">
-        <v>0.5503285851377906</v>
+        <v>0.6319878365234823</v>
       </c>
       <c r="K1" t="n">
-        <v>0.5810571285231321</v>
+        <v>0.799061303763383</v>
       </c>
       <c r="L1" t="n">
-        <v>0.5966706443505249</v>
+        <v>0.6560588825523056</v>
       </c>
       <c r="M1" t="n">
-        <v>0.04336581807008101</v>
+        <v>0.1177474474192239</v>
       </c>
       <c r="N1" t="n">
-        <v>0.009679760335245978</v>
+        <v>0.2879516253165925</v>
       </c>
       <c r="O1" t="n">
-        <v>0.8299091677585522</v>
+        <v>0.6800990368302656</v>
       </c>
       <c r="P1" t="n">
-        <v>0.6813929303603886</v>
+        <v>0.004373669065717612</v>
       </c>
       <c r="Q1" t="n">
-        <v>0.243718345217564</v>
+        <v>0.5513279371294626</v>
       </c>
       <c r="R1" t="n">
-        <v>0.6933683016170096</v>
+        <v>0.0001786393149179287</v>
       </c>
       <c r="S1" t="n">
-        <v>0.01961249510953438</v>
+        <v>0.007915089335447351</v>
       </c>
       <c r="T1" t="n">
-        <v>0.297262807367821</v>
+        <v>0.2875377601078369</v>
       </c>
       <c r="U1" t="n">
-        <v>0.3860751993388274</v>
+        <v>0.0070319754608143</v>
       </c>
       <c r="V1" t="n">
-        <v>0.8808904663625907</v>
+        <v>0.4518882736233095</v>
       </c>
       <c r="W1" t="n">
-        <v>0.8860284233338943</v>
+        <v>0.2778554665154102</v>
       </c>
       <c r="X1" t="n">
-        <v>0.5777324186857782</v>
+        <v>0.3721994913173508</v>
       </c>
       <c r="Y1" t="n">
-        <v>0.4999981411578343</v>
+        <v>0.5799295172998659</v>
       </c>
       <c r="Z1" t="n">
-        <v>0.00106721709442823</v>
+        <v>0.003294461839891509</v>
       </c>
       <c r="AA1" t="n">
-        <v>0.03141655975048346</v>
+        <v>0.03885444649476023</v>
       </c>
       <c r="AB1" t="n">
-        <v>0.3750645325109596</v>
+        <v>0.4111553952455109</v>
       </c>
       <c r="AC1" t="n">
-        <v>0.2623583896403122</v>
+        <v>0.7818987283349808</v>
       </c>
     </row>
     <row r="2">
@@ -780,88 +780,88 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.003265055510172715</v>
+        <v>0.02375043742969527</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1106549297250164</v>
+        <v>0.1073572271793384</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2127046296797881</v>
+        <v>0.2067849033913336</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05056830372993838</v>
+        <v>0.04766549373645818</v>
       </c>
       <c r="F2" t="n">
-        <v>0.001590063818718404</v>
+        <v>0.001630250093145511</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04926330096213603</v>
+        <v>0.04553711226085804</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1881639992941448</v>
+        <v>0.1859859845545214</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5974922061853769</v>
+        <v>0.5964220914094107</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8447179358059413</v>
+        <v>0.8387939777811376</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4994698333320897</v>
+        <v>0.5095237825369723</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5798395646490719</v>
+        <v>0.5732824205408686</v>
       </c>
       <c r="M2" t="n">
-        <v>0.042924402895097</v>
+        <v>0.04331917708020284</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9553671885346766</v>
+        <v>0.9224982834310611</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1048321424592351</v>
+        <v>0.1051921292270367</v>
       </c>
       <c r="P2" t="n">
-        <v>0.2959970676638896</v>
+        <v>0.3642611122348743</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.327997516422892</v>
+        <v>0.3434480757402509</v>
       </c>
       <c r="R2" t="n">
-        <v>0.91827277649437</v>
+        <v>0.891055936457596</v>
       </c>
       <c r="S2" t="n">
-        <v>0.009384197623856342</v>
+        <v>0.008314958177436054</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7368050028327899</v>
+        <v>0.7470198061058191</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8189795086019916</v>
+        <v>0.9185833435084131</v>
       </c>
       <c r="V2" t="n">
-        <v>0.4339595627402305</v>
+        <v>0.4310305040180122</v>
       </c>
       <c r="W2" t="n">
-        <v>0.7512326106562067</v>
+        <v>0.7507388546658559</v>
       </c>
       <c r="X2" t="n">
-        <v>0.1644651945960204</v>
+        <v>0.1615298508565926</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.329066535130667</v>
+        <v>0.3297530858597806</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.5261732865469213</v>
+        <v>0.5198003528585318</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.1911141713146485</v>
+        <v>0.1834255894586183</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.778542506435159</v>
+        <v>0.7896326947511075</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.4742819917075867</v>
+        <v>0.4948963109313614</v>
       </c>
     </row>
     <row r="3">
@@ -871,88 +871,88 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9640035125439661</v>
+        <v>0.5244635428068976</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4260621898296368</v>
+        <v>0.4833578709185503</v>
       </c>
       <c r="D3" t="n">
-        <v>0.428822781900299</v>
+        <v>0.4945863166239952</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7941964312149804</v>
+        <v>0.7392169627053686</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8762415887837184</v>
+        <v>0.7700725278547405</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5815522684298395</v>
+        <v>0.5417686205047205</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9877927780284984</v>
+        <v>0.9592899506349364</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1599583100975382</v>
+        <v>0.1918495114186566</v>
       </c>
       <c r="J3" t="n">
-        <v>0.05658980012935177</v>
+        <v>0.05999013637522568</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4841058688108639</v>
+        <v>0.5318941978197615</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5781498787329327</v>
+        <v>0.5182424825967915</v>
       </c>
       <c r="M3" t="n">
-        <v>0.6223744155842419</v>
+        <v>0.7368435568380391</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9957605106919489</v>
+        <v>0.6819007309191556</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1119958327684205</v>
+        <v>0.07651620282420128</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4461880986062152</v>
+        <v>0.1742364844355967</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.7869170799582227</v>
+        <v>0.5439639760167427</v>
       </c>
       <c r="R3" t="n">
-        <v>0.4976562836481941</v>
+        <v>0.3499262522411721</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9159569205715863</v>
+        <v>0.9879805070976364</v>
       </c>
       <c r="T3" t="n">
-        <v>0.03736579608999685</v>
+        <v>0.04553170347304514</v>
       </c>
       <c r="U3" t="n">
-        <v>0.07131684105444486</v>
+        <v>0.1359252229724406</v>
       </c>
       <c r="V3" t="n">
-        <v>0.3332081304278209</v>
+        <v>0.5184413777611927</v>
       </c>
       <c r="W3" t="n">
-        <v>0.1342240828412485</v>
+        <v>0.2512783321987999</v>
       </c>
       <c r="X3" t="n">
-        <v>0.9380949223214059</v>
+        <v>0.9232696201353147</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.6802052078125447</v>
+        <v>0.6002129334558687</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.1478019220793385</v>
+        <v>0.1117077736217082</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.9720865546323418</v>
+        <v>0.9742033261554052</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.02959946087332164</v>
+        <v>0.02735232514285601</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.8213682588267391</v>
+        <v>0.6161221705900495</v>
       </c>
     </row>
     <row r="4">
@@ -962,88 +962,88 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2212291972766952</v>
+        <v>0.3999929792663647</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5170814158277903</v>
+        <v>0.5948492503645508</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4337627947003037</v>
+        <v>0.5009214037373009</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6092813841027378</v>
+        <v>0.5008845239934936</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3907278508729536</v>
+        <v>0.4348552374385555</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3625181420670707</v>
+        <v>0.274347571350979</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1709405242633848</v>
+        <v>0.1533272998406763</v>
       </c>
       <c r="I4" t="n">
-        <v>0.03536957667494211</v>
+        <v>0.04739015087125187</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5904700193519276</v>
+        <v>0.6101441316730711</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3573485396158953</v>
+        <v>0.3575967755612792</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7401403148579703</v>
+        <v>0.850797150307895</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3461835039320315</v>
+        <v>0.3746069718001762</v>
       </c>
       <c r="N4" t="n">
-        <v>0.5332044968972034</v>
+        <v>0.4831986327906239</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2149829931641168</v>
+        <v>0.2714807508987917</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9348048983711559</v>
+        <v>0.7634342598949686</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.2241684037163882</v>
+        <v>0.325910639393034</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1486266075353213</v>
+        <v>0.9511492261849811</v>
       </c>
       <c r="S4" t="n">
-        <v>0.5692553267629388</v>
+        <v>0.4295554436179833</v>
       </c>
       <c r="T4" t="n">
-        <v>0.3576820396016221</v>
+        <v>0.5093743523061263</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8180409421919164</v>
+        <v>0.4459791346892137</v>
       </c>
       <c r="V4" t="n">
-        <v>0.0006484124470979099</v>
+        <v>0.001850378147133524</v>
       </c>
       <c r="W4" t="n">
-        <v>0.1633921210684707</v>
+        <v>0.3099528511930414</v>
       </c>
       <c r="X4" t="n">
-        <v>0.02414048365719993</v>
+        <v>0.04465472538891131</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.3669311631354204</v>
+        <v>0.4644671381394591</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.4062644307223741</v>
+        <v>0.3826941805193546</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.7578677102589477</v>
+        <v>0.8667734416878273</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.6337289505338631</v>
+        <v>0.548069743751868</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.06340052079026333</v>
+        <v>0.1008714083551703</v>
       </c>
     </row>
     <row r="5">
@@ -1053,88 +1053,88 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5712854167047814</v>
+        <v>0.9676879151660709</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7228387288997749</v>
+        <v>0.8214966880894973</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9863038455225523</v>
+        <v>0.88698264727557</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5182978349784975</v>
+        <v>0.5678818407252302</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8627420246627254</v>
+        <v>0.8387188959406575</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4960961567290284</v>
+        <v>0.5604100332889874</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6399013374088641</v>
+        <v>0.6174231498603775</v>
       </c>
       <c r="I5" t="n">
-        <v>0.406660464088103</v>
+        <v>0.4156261258701593</v>
       </c>
       <c r="J5" t="n">
-        <v>0.08922687453742531</v>
+        <v>0.09591515289381763</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0007692005853912367</v>
+        <v>0.000959474777527617</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7204247932619603</v>
+        <v>0.7593440963481732</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2222761217417651</v>
+        <v>0.2521246494872548</v>
       </c>
       <c r="N5" t="n">
-        <v>0.649143330060544</v>
+        <v>0.779391731382441</v>
       </c>
       <c r="O5" t="n">
-        <v>0.776395457568122</v>
+        <v>0.757536118087424</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4843772407172749</v>
+        <v>0.469486688053309</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.5293357190659476</v>
+        <v>0.7736265417723436</v>
       </c>
       <c r="R5" t="n">
-        <v>0.5172123865317557</v>
+        <v>0.6274156757839338</v>
       </c>
       <c r="S5" t="n">
-        <v>0.7165816541509551</v>
+        <v>0.781672554571489</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8733979972674535</v>
+        <v>0.7770169236363826</v>
       </c>
       <c r="U5" t="n">
-        <v>0.007000171785162508</v>
+        <v>0.04070206783086376</v>
       </c>
       <c r="V5" t="n">
-        <v>0.4976309813411239</v>
+        <v>0.5010823966092123</v>
       </c>
       <c r="W5" t="n">
-        <v>0.4312063865362863</v>
+        <v>0.3909928104655345</v>
       </c>
       <c r="X5" t="n">
-        <v>0.5803595205944092</v>
+        <v>0.6392350295824976</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.8653398256772349</v>
+        <v>0.9112744399661284</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.5432067663651384</v>
+        <v>0.5172361175489117</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3876726578036593</v>
+        <v>0.4445103702346217</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.07064059421984227</v>
+        <v>0.08301711590572375</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.02923613649361611</v>
+        <v>0.03572016107851608</v>
       </c>
     </row>
     <row r="6">
@@ -1144,88 +1144,88 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06527397259984592</v>
+        <v>0.3147774005691378</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4115692493364356</v>
+        <v>0.429867423377859</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2946468541100222</v>
+        <v>0.3161471218721142</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9104270929220013</v>
+        <v>0.9802431286901653</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8712900127353467</v>
+        <v>0.7949481060878767</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9830990686534808</v>
+        <v>0.9492069433488077</v>
       </c>
       <c r="H6" t="n">
-        <v>0.01227687758940414</v>
+        <v>0.01099640448253675</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1268930845262476</v>
+        <v>0.1514749943148615</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6818466595001957</v>
+        <v>0.6903284920472303</v>
       </c>
       <c r="K6" t="n">
-        <v>0.09377535063480683</v>
+        <v>0.08803560465058113</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3938563810147417</v>
+        <v>0.3440693855700289</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4631299197313534</v>
+        <v>0.4102139721778172</v>
       </c>
       <c r="N6" t="n">
-        <v>0.03450505407220683</v>
+        <v>0.02590616505808611</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8909695336073196</v>
+        <v>0.7750633966063002</v>
       </c>
       <c r="P6" t="n">
-        <v>0.0004255636061791559</v>
+        <v>0.01874569565963307</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.3061699032611666</v>
+        <v>0.4656361669192324</v>
       </c>
       <c r="R6" t="n">
-        <v>0.4162220701871842</v>
+        <v>0.5689375195711009</v>
       </c>
       <c r="S6" t="n">
-        <v>0.8152665196999658</v>
+        <v>0.7105582192675013</v>
       </c>
       <c r="T6" t="n">
-        <v>0.4442389783156685</v>
+        <v>0.5306707964129846</v>
       </c>
       <c r="U6" t="n">
-        <v>0.4531145559021782</v>
+        <v>0.498652537551637</v>
       </c>
       <c r="V6" t="n">
-        <v>0.1605242887898985</v>
+        <v>0.1007587305762192</v>
       </c>
       <c r="W6" t="n">
-        <v>0.1572849019401996</v>
+        <v>0.08001220489750734</v>
       </c>
       <c r="X6" t="n">
-        <v>0.9416885255047187</v>
+        <v>0.7996792698424573</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6778474339178171</v>
+        <v>0.7602352039454956</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.6846642663883388</v>
+        <v>0.7699244417042836</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.3103045681885166</v>
+        <v>0.2925175752066057</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.8270614749251143</v>
+        <v>0.8650224610367561</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.5544840447543218</v>
+        <v>0.4291683765846607</v>
       </c>
     </row>
     <row r="7">
@@ -1235,88 +1235,88 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1500472598266012</v>
+        <v>0.2920738398956164</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4074417300031881</v>
+        <v>0.3821186781828541</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3129448864184115</v>
+        <v>0.2961824452321424</v>
       </c>
       <c r="E7" t="n">
-        <v>0.899500948321257</v>
+        <v>0.8250128038368095</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7672849541759004</v>
+        <v>0.7999982958413765</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4843006155690804</v>
+        <v>0.5507760028078186</v>
       </c>
       <c r="H7" t="n">
-        <v>0.005845637177632453</v>
+        <v>0.005273481513422687</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0199727071538817</v>
+        <v>0.02375509866323905</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8377270749885881</v>
+        <v>0.8475769778906495</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3246616504423075</v>
+        <v>0.3305100402424808</v>
       </c>
       <c r="L7" t="n">
-        <v>0.3516652517904844</v>
+        <v>0.3105806739543174</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1534101637245241</v>
+        <v>0.1525650036098221</v>
       </c>
       <c r="N7" t="n">
-        <v>0.5997110645370511</v>
+        <v>0.5691331002821014</v>
       </c>
       <c r="O7" t="n">
-        <v>0.6771600955086249</v>
+        <v>0.7342952495835778</v>
       </c>
       <c r="P7" t="n">
-        <v>0.07062611121643603</v>
+        <v>0.2173008249142101</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.5320232610366595</v>
+        <v>0.5471365870705251</v>
       </c>
       <c r="R7" t="n">
-        <v>0.4071430167834944</v>
+        <v>0.9507628517226795</v>
       </c>
       <c r="S7" t="n">
-        <v>0.9617024214371959</v>
+        <v>0.9367396222074451</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1026208363917178</v>
+        <v>0.1327674316456441</v>
       </c>
       <c r="U7" t="n">
-        <v>0.209107124600082</v>
+        <v>0.3787835422891311</v>
       </c>
       <c r="V7" t="n">
-        <v>0.299270981996213</v>
+        <v>0.2406395760716554</v>
       </c>
       <c r="W7" t="n">
-        <v>0.4030796195996157</v>
+        <v>0.2862038385418413</v>
       </c>
       <c r="X7" t="n">
-        <v>0.6703385182613515</v>
+        <v>0.7824933722943163</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.4283711900401495</v>
+        <v>0.4857611711927247</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.2469722016123294</v>
+        <v>0.2689025544097206</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.8760462404355179</v>
+        <v>0.8155493050479717</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.8610326532128025</v>
+        <v>0.9183170976521671</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.5754826856733275</v>
+        <v>0.6554750885270628</v>
       </c>
     </row>
     <row r="8">
@@ -1326,88 +1326,88 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.3545576852648015</v>
+        <v>0.9443383482867785</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6731635043871039</v>
+        <v>0.5858933505037465</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4377534901301984</v>
+        <v>0.3662591951160222</v>
       </c>
       <c r="E8" t="n">
-        <v>0.940313567774679</v>
+        <v>0.9311913975106135</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7786458684631603</v>
+        <v>0.6944701950873378</v>
       </c>
       <c r="G8" t="n">
-        <v>0.7574931348505228</v>
+        <v>0.7645170108249275</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4079151900780285</v>
+        <v>0.4109860270975422</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1008337533374363</v>
+        <v>0.08667143397342668</v>
       </c>
       <c r="J8" t="n">
-        <v>0.4110449075410135</v>
+        <v>0.4303273316131095</v>
       </c>
       <c r="K8" t="n">
-        <v>0.05824050314150171</v>
+        <v>0.0688745187157094</v>
       </c>
       <c r="L8" t="n">
-        <v>0.48739459000706</v>
+        <v>0.4621730912798216</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1332095544029948</v>
+        <v>0.1753037957168214</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8758394479781167</v>
+        <v>0.8285841000516045</v>
       </c>
       <c r="O8" t="n">
-        <v>0.6706890735898017</v>
+        <v>0.5648453383681572</v>
       </c>
       <c r="P8" t="n">
-        <v>0.4560050015574264</v>
+        <v>0.2276362937039207</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.0316315409366574</v>
+        <v>0.02050809752179084</v>
       </c>
       <c r="R8" t="n">
-        <v>0.871631580241908</v>
+        <v>0.369542789711911</v>
       </c>
       <c r="S8" t="n">
-        <v>0.9657686082896988</v>
+        <v>0.9317704094593311</v>
       </c>
       <c r="T8" t="n">
-        <v>0.448843222145406</v>
+        <v>0.4225802506203196</v>
       </c>
       <c r="U8" t="n">
-        <v>0.1923263179575458</v>
+        <v>0.4064499980917354</v>
       </c>
       <c r="V8" t="n">
-        <v>0.06381687999387342</v>
+        <v>0.1040709305522606</v>
       </c>
       <c r="W8" t="n">
-        <v>0.6744758265471376</v>
+        <v>0.8465158125267154</v>
       </c>
       <c r="X8" t="n">
-        <v>0.2563533543750572</v>
+        <v>0.2806749194939911</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.8196856056781543</v>
+        <v>0.8551818883372211</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.8403937695881082</v>
+        <v>0.738988354175136</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1843117391326698</v>
+        <v>0.1988861789336525</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.7029533764570868</v>
+        <v>0.719371173046943</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.6018679874780418</v>
+        <v>0.4656816127412289</v>
       </c>
     </row>
     <row r="9">
@@ -1417,88 +1417,88 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.03552379185870463</v>
+        <v>0.2949644561064799</v>
       </c>
       <c r="C9" t="n">
-        <v>0.911332343405681</v>
+        <v>0.9337071674032518</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8248826794835201</v>
+        <v>0.8599402608134002</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5834817795090077</v>
+        <v>0.6802083169798261</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6930037087091918</v>
+        <v>0.5914073786478635</v>
       </c>
       <c r="G9" t="n">
-        <v>0.411798117805418</v>
+        <v>0.490312549554049</v>
       </c>
       <c r="H9" t="n">
-        <v>0.001895512532837737</v>
+        <v>0.001597629313706152</v>
       </c>
       <c r="I9" t="n">
-        <v>0.02055732973282794</v>
+        <v>0.02975452795577371</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6330379611883219</v>
+        <v>0.6446077615757557</v>
       </c>
       <c r="K9" t="n">
-        <v>0.188883846247992</v>
+        <v>0.1742351287832699</v>
       </c>
       <c r="L9" t="n">
-        <v>0.2253886601268431</v>
+        <v>0.1765913661516325</v>
       </c>
       <c r="M9" t="n">
-        <v>0.4518829334361011</v>
+        <v>0.3761387669549556</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2468684564590886</v>
+        <v>0.140210701137859</v>
       </c>
       <c r="O9" t="n">
-        <v>0.6444945655250567</v>
+        <v>0.4979578834236228</v>
       </c>
       <c r="P9" t="n">
-        <v>0.004018707367806075</v>
+        <v>0.1228597871027327</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.615259971812975</v>
+        <v>0.8522735923865354</v>
       </c>
       <c r="R9" t="n">
-        <v>0.2072102244907419</v>
+        <v>0.411791272203058</v>
       </c>
       <c r="S9" t="n">
-        <v>0.6143233187218253</v>
+        <v>0.7649089314321303</v>
       </c>
       <c r="T9" t="n">
-        <v>0.04862447381392675</v>
+        <v>0.07691511411077033</v>
       </c>
       <c r="U9" t="n">
-        <v>0.2352203495980102</v>
+        <v>0.299931510054451</v>
       </c>
       <c r="V9" t="n">
-        <v>0.3233782172535661</v>
+        <v>0.174923617670891</v>
       </c>
       <c r="W9" t="n">
-        <v>0.3588243869753137</v>
+        <v>0.1565661239306563</v>
       </c>
       <c r="X9" t="n">
-        <v>0.4916842570214499</v>
+        <v>0.6742848174792522</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.4672785488050419</v>
+        <v>0.5777892907425948</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.5213777440503362</v>
+        <v>0.6368895265167711</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.8623271858122347</v>
+        <v>0.8131471594033386</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.7440805197903139</v>
+        <v>0.8044233213985293</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.2881942385172418</v>
+        <v>0.1771085863011277</v>
       </c>
     </row>
     <row r="10">
@@ -1508,88 +1508,88 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1200833457189325</v>
+        <v>0.3094872731771856</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2535861644640119</v>
+        <v>0.2520074025754242</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1900489745920208</v>
+        <v>0.1921585863944154</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6999501416165799</v>
+        <v>0.6463965629424349</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7079541950071176</v>
+        <v>0.7491882889506203</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9525727771934411</v>
+        <v>0.9874266468652719</v>
       </c>
       <c r="H10" t="n">
-        <v>0.007227564248221172</v>
+        <v>0.006616441238185343</v>
       </c>
       <c r="I10" t="n">
-        <v>0.04788338244717909</v>
+        <v>0.05501191355266509</v>
       </c>
       <c r="J10" t="n">
-        <v>0.7322967498115214</v>
+        <v>0.7339787541745466</v>
       </c>
       <c r="K10" t="n">
-        <v>0.2316192305345577</v>
+        <v>0.2296059328048606</v>
       </c>
       <c r="L10" t="n">
-        <v>0.3220095730979029</v>
+        <v>0.2891170290479038</v>
       </c>
       <c r="M10" t="n">
-        <v>0.3041084362314609</v>
+        <v>0.2894522194750258</v>
       </c>
       <c r="N10" t="n">
-        <v>0.2935648934700439</v>
+        <v>0.2692914885099787</v>
       </c>
       <c r="O10" t="n">
-        <v>0.7974510233154943</v>
+        <v>0.8648820522586941</v>
       </c>
       <c r="P10" t="n">
-        <v>0.006082724587204545</v>
+        <v>0.05189154150701456</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.3818594096547776</v>
+        <v>0.4618071378665169</v>
       </c>
       <c r="R10" t="n">
-        <v>0.5206905958838728</v>
+        <v>0.8206283842248843</v>
       </c>
       <c r="S10" t="n">
-        <v>0.6314423352470668</v>
+        <v>0.5574622262168101</v>
       </c>
       <c r="T10" t="n">
-        <v>0.2730722497249047</v>
+        <v>0.3199237717568554</v>
       </c>
       <c r="U10" t="n">
-        <v>0.3291570266640141</v>
+        <v>0.4363721211989354</v>
       </c>
       <c r="V10" t="n">
-        <v>0.09886967847624561</v>
+        <v>0.07450600023249027</v>
       </c>
       <c r="W10" t="n">
-        <v>0.1637737737863772</v>
+        <v>0.1065009152308788</v>
       </c>
       <c r="X10" t="n">
-        <v>0.8510085176512774</v>
+        <v>0.9516500165764606</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.5006020871664975</v>
+        <v>0.5516217434159654</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.5484288458821769</v>
+        <v>0.5899499432740904</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.7405248155782722</v>
+        <v>0.7055047782757722</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.4528350832777417</v>
+        <v>0.481710920557384</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.5654625796273958</v>
+        <v>0.656552095682948</v>
       </c>
     </row>
     <row r="11">
@@ -1599,88 +1599,88 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2932119518015475</v>
+        <v>0.6754171934012092</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3231392623804752</v>
+        <v>0.4142713070739761</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2691426986776804</v>
+        <v>0.3497490153605298</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4762786237246357</v>
+        <v>0.5697041577715707</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2035117213010891</v>
+        <v>0.2098522125002719</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8139809380427941</v>
+        <v>0.952289293605834</v>
       </c>
       <c r="H11" t="n">
-        <v>0.559030928414487</v>
+        <v>0.5211712382010933</v>
       </c>
       <c r="I11" t="n">
-        <v>0.824120793924194</v>
+        <v>0.8733601830188018</v>
       </c>
       <c r="J11" t="n">
-        <v>0.02020801372474004</v>
+        <v>0.02329810459796782</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3018286730426317</v>
+        <v>0.3309088387704531</v>
       </c>
       <c r="L11" t="n">
-        <v>0.4475633053467197</v>
+        <v>0.5176291460227789</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2978887751143373</v>
+        <v>0.2891307398793641</v>
       </c>
       <c r="N11" t="n">
-        <v>0.03493665705805638</v>
+        <v>0.04547812825201766</v>
       </c>
       <c r="O11" t="n">
-        <v>0.02121077326648397</v>
+        <v>0.0251370760856921</v>
       </c>
       <c r="P11" t="n">
-        <v>0.6068745877746162</v>
+        <v>0.7012224860521469</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.2837042588064748</v>
+        <v>0.5023770593460513</v>
       </c>
       <c r="R11" t="n">
-        <v>0.2192036336134589</v>
+        <v>0.6925659826273691</v>
       </c>
       <c r="S11" t="n">
-        <v>0.5989606285513209</v>
+        <v>0.7272434963618692</v>
       </c>
       <c r="T11" t="n">
-        <v>0.3655444891876464</v>
+        <v>0.4923074357986774</v>
       </c>
       <c r="U11" t="n">
-        <v>0.03113051267870156</v>
+        <v>0.1829672187658536</v>
       </c>
       <c r="V11" t="n">
-        <v>0.6474802872358385</v>
+        <v>0.5710568937525544</v>
       </c>
       <c r="W11" t="n">
-        <v>0.7168049688742888</v>
+        <v>0.8941637735836978</v>
       </c>
       <c r="X11" t="n">
-        <v>0.6166802920917143</v>
+        <v>0.7623746243058332</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.434338293951347</v>
+        <v>0.5135954764350981</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.1736131028729024</v>
+        <v>0.184813924132411</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.9141722804483261</v>
+        <v>0.9648845223308065</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.5692625941879466</v>
+        <v>0.6608918047964716</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.7938968967303132</v>
+        <v>0.7665686816997782</v>
       </c>
     </row>
   </sheetData>
@@ -1709,7 +1709,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.1314353532120548</v>
+        <v>0.2435296378992828</v>
       </c>
     </row>
     <row r="3">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1607302509912042</v>
+        <v>0.1641786527814016</v>
       </c>
     </row>
     <row r="4">
@@ -1729,7 +1729,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1716009923511378</v>
+        <v>0.1542563859870855</v>
       </c>
     </row>
     <row r="5">
@@ -1739,7 +1739,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1898313285451632</v>
+        <v>0.188347773887227</v>
       </c>
     </row>
     <row r="6">
@@ -1749,7 +1749,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2260255802634429</v>
+        <v>0.2234298584390778</v>
       </c>
     </row>
     <row r="7">
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.106789534125648</v>
+        <v>0.1006958590885076</v>
       </c>
     </row>
     <row r="8">
@@ -1769,7 +1769,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2531958974603025</v>
+        <v>0.2589627628479452</v>
       </c>
     </row>
     <row r="9">
@@ -1779,7 +1779,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1346273810804107</v>
+        <v>0.1266937968775598</v>
       </c>
     </row>
     <row r="10">
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1931755423556811</v>
+        <v>0.1902712956619745</v>
       </c>
     </row>
     <row r="11">
@@ -1799,7 +1799,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1667515480541235</v>
+        <v>0.1554560065858979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>